<commit_message>
update strategy settings for day trading
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,39 +95,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1. 更新so，设1手
 2. f50需更新ev文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>日盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">郑州日盘的so，如果今天晚上正常，明天部署
 BDY 2017/1/3 19:57:46
 日盘手数暂定如下：
-ta fl34 3
-zc fl34 1
-ma fl34 5
-sr fl36 1
-cf fl36 1
-ta fl36 1
-zc fl36 1
-cf fw10 1
-ta fw10 3
-zc fw10 2
-zc fd10 2
-ta fd10 3
+(ok) ta fl34 3
+(ok) zc fl34 1
+(ok) ma fl34 5
+(ok) sr fl36 1
+(ok) cf fl36 1
+(ok) ta fl36 1
+(ok) zc fl36 1
+(ok) cf fw10 1
+(ok) ta fw10 3
+(ok) zc fw10 2
+(ok) zc fd10 2
+(ok) ta fd10 3
 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -574,7 +570,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -638,10 +634,10 @@
         <v>42738</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="229.5">
@@ -649,13 +645,13 @@
         <v>10</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="7">
         <v>42738</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F5" s="12" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
update strategy settings for dce
暂定手数
(ok) dlm fl34 1
(ok) dla fl34 2
(ok) dljd fl34 3
(ok) dli fl34 40
(ok) dlv fl34 6
(ok) dlv fl36 3
(oK) dlm fl36 3
(ok) dla fl36 2
(ok) dljd fl36 1
(ok) dli fl36 20
(ok) dlv fw10 3
(ok) dla fw10 2
(ok) dla fd10 1
(ok) dll fd10 1
(ok) dljd fd10 1
2。先把铁矿手数减半，我怕钱不够用
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -100,36 +100,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>pending</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大连</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>日盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">暂定手数
-dlm fl34 1
-dla fl34 2
-dljd fl34 3
-dli fl34 40
-dlv fl34 6
-dlv fl36 3
-dlm fl36 3
-dla fl36 2
-dljd fl36 1
-dli fl36 20
-dlv fw10 3
-dla fw10 2
-dla fd10 1
-dll fd10 1
-dljd fd10 1
-2。先把铁矿手数减半，我怕钱不够用
-</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -202,6 +177,27 @@
   </si>
   <si>
     <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">暂定手数
+(ok) dlm fl34 1
+(ok) dla fl34 2
+(ok) dljd fl34 3
+(ok) dli fl34 40
+(ok) dlv fl34 6
+(ok) dlv fl36 3
+(oK) dlm fl36 3
+(ok) dla fl36 2
+(ok) dljd fl36 1
+(ok) dli fl36 20
+(ok) dlv fw10 3
+(ok) dla fw10 2
+(ok) dla fd10 1
+(ok) dll fd10 1
+(ok) dljd fd10 1
+2。先把铁矿手数减半，我怕钱不够用
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -687,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -752,27 +748,27 @@
         <v>42739</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="273.60000000000002" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="7">
         <v>41643</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update strategy so files and settings
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,16 +87,120 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>夜盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>郑州</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>夜盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1. 更新so，设1手
-2. f50需更新ev文件</t>
+    <t>更新fl50 ev文件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(ok) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(1) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新上期夜盘所有策略so，</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(2)设定手数</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">:total:41
+sh_night
+(ok) ni fl35 1
+(ok) ni fd10 2
+(ok) pb fl34 1
+(ok) pb fl35 1
+(ok) pb fw10 1
+(ok) pb fd10 2
+(ok) zn fl34 3
+(ok) zn fl36 2
+(ok) zn fd10 3
+(ok) ru fl34 2
+(ok) ru fl36 2
+(ok) ru fd10 1
+(oK) al fl34 1
+(ok) al fw10 1
+(ok) ag fl34 1
+(ok) ag fd10 4
+(ok) au fl34 2
+(ok) au fl36 2
+(ok) au fd10 2
+(ok) hc fl34 2
+(ok) hc fl36 2
+(ok) hc fd10 2
+(ok) cu fd10 1
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -104,26 +208,162 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">郑州日盘的so，如果今天晚上正常，明天部署
-BDY 2017/1/3 19:57:46
-日盘手数暂定如下：
-(ok) ta fl34 3
-(ok) zc fl34 1
-(ok) ma fl34 5
-(ok) sr fl36 1
-(ok) cf fl36 1
-(ok) ta fl36 1
-(ok) zc fl36 1
-(ok) cf fw10 1
-(ok) ta fw10 3
-(ok) zc fw10 2
-(ok) zc fd10 2
-(ok) ta fd10 3
+    <r>
+      <t xml:space="preserve">1. (ok) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新上期所日盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>fl34</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>策略的</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">so
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>其它非</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>fl34</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">策略使用原来配置
 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>设定日盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>fl34</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">手数：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">sh_day
+(ok) ni fl34 1
+(ok) ru fl34 2
+(ok) ag fl34 2
+(ok) zn fl34 3
+(ok) al fl34 1
+(ok) pb fl34 1
+(ok) hc fl34 2
+(ok) au fl34 3
+(ok) 3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>合约换月</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -264,8 +504,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F14" totalsRowShown="0">
-  <autoFilter ref="A2:F14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F12" totalsRowShown="0">
+  <autoFilter ref="A2:F12">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
@@ -567,20 +807,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="8" style="10" customWidth="1"/>
-    <col min="2" max="2" width="8.375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="7.875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="10" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.25" style="11" customWidth="1"/>
+    <col min="2" max="2" width="6.375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="6.25" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="7.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.375" style="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="2.25" customHeight="1">
@@ -623,50 +863,56 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="34.5" customHeight="1">
+    <row r="4" spans="1:6" ht="48" customHeight="1">
       <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="7">
+        <v>42374</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="7">
-        <v>42738</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="33.75" customHeight="1">
+      <c r="B5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="7">
+        <v>42374</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="12" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="5" spans="1:6" ht="229.5">
-      <c r="B5" s="6" t="s">
+    <row r="6" spans="1:6" ht="213.75">
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>42009</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="7">
-        <v>42738</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="75.75" customHeight="1">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="F7" s="12"/>
+      <c r="F6" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update shfe strategy so files for day trading
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -87,26 +87,17 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>上期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>夜盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>郑州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新fl50 ev文件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
+    <t>日盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(ok) (1) </t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -115,7 +106,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">(ok) </t>
+      <t>继续更新日盘上期策略</t>
     </r>
     <r>
       <rPr>
@@ -125,7 +116,8 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">(1) </t>
+      <t xml:space="preserve">so:
+(2) </t>
     </r>
     <r>
       <rPr>
@@ -135,7 +127,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>更新上期夜盘所有策略so，</t>
+      <t>和上次的</t>
     </r>
     <r>
       <rPr>
@@ -145,8 +137,7 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">
-</t>
+      <t>fl34</t>
     </r>
     <r>
       <rPr>
@@ -156,7 +147,9 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>(2)设定手数</t>
+      <t xml:space="preserve">一起：
+日盘参数：
+</t>
     </r>
     <r>
       <rPr>
@@ -166,204 +159,38 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">:total:41
-sh_night
-(ok) ni fl35 1
-(ok) ni fd10 2
-(ok) pb fl34 1
-(ok) pb fl35 1
-(ok) pb fw10 1
-(ok) pb fd10 2
-(ok) zn fl34 3
-(ok) zn fl36 2
-(ok) zn fd10 3
-(ok) ru fl34 2
-(ok) ru fl36 2
-(ok) ru fd10 1
-(oK) al fl34 1
-(ok) al fw10 1
-(ok) ag fl34 1
-(ok) ag fd10 4
-(ok) au fl34 2
-(ok) au fl36 2
-(ok) au fd10 2
-(ok) hc fl34 2
-(ok) hc fl36 2
-(ok) hc fd10 2
-(ok) cu fd10 1
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. (ok) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新上期所日盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>fl34</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>策略的</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">so
-   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>其它非</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>fl34</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">策略使用原来配置
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>设定日盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>fl34</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">手数：
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">sh_day
-(ok) ni fl34 1
+      <t xml:space="preserve">(ok) ni fl34 1
 (ok) ru fl34 2
 (ok) ag fl34 2
-(ok) zn fl34 3
+(ok) zn fl34 1
 (ok) al fl34 1
 (ok) pb fl34 1
 (ok) hc fl34 2
 (ok) au fl34 3
-(ok) 3. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>合约换月</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+(ok) ni fd10 1
+(ok) ru fd10 1
+(ok) zn fd10 1
+(ok) pb fd10 1
+(ok) ni fl35 1
+(ok) pb fl35 1
+(ok) ru fl36 2
+(ok) ag fl36 2
+(ok) zn fl36 1
+(ok) al fl36 1
+(ok) au fl36 2
+(ok) ni fw10 1
+(ok) ru fw10 2
+(ok) ag fw10 2
+(ok) zn fw10 1
+(ok) al fw10 1
+(ok) au fw10 1
+(ok) pb fw10 1
 </t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -504,8 +331,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F12" totalsRowShown="0">
-  <autoFilter ref="A2:F12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F9" totalsRowShown="0">
+  <autoFilter ref="A2:F9">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
@@ -807,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -863,55 +690,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="48" customHeight="1">
+    <row r="4" spans="1:6" ht="175.5" customHeight="1">
       <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="7">
+        <v>42743</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="7">
-        <v>42374</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="33.75" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="7">
-        <v>42374</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="213.75">
-      <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="7">
-        <v>42009</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update stategy setting for czce night trading
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -97,67 +97,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>更新夜盘f50 ev文件</t>
+    <t>更新夜盘ev文件</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>夜盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">调整一下夜盘的手数，上期
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">sh_night
-(ok) ni fl35 1
-(ok) ni fd10 1
-(ok) pb fl34 1
-(ok) pb fl35 1
-(ok) pb fw10 1
-(ok) pb fd10 1
-(ok) zn fl34 1
-(ok) zn fl36 1
-(ok) zn fd10 1
-(ok) ru fl34 2
-(ok) ru fl36 2
-(ok) ru fd10 1
-(ok) al fl34 1
-(ok) al fw10 1
-(ok) ag fl34 1
-(ok) ag fd10 4
-(ok) au fl34 2
-(ok) au fl36 2
-(ok) au fd10 2
-(ok) hc fl34 2
-(ok) hc fl36 2
-(ok) hc fd10 2
-(ok) cu fd10 1
-</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -603,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -665,7 +609,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="7">
-        <v>42744</v>
+        <v>42745</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -674,22 +618,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="369.75">
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7">
-        <v>42744</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>16</v>
-      </c>
+    <row r="5" spans="1:6">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update strategy so files and settings for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -288,15 +288,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>：w</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>上期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>夜盘</t>
+    <t>状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>郑州</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -304,52 +300,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>上期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>日盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>郑州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>夜盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新fl33系列 so
-2.更新ev
-3.每个合约1手</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>85</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>账户，fl50,fl51：更新</t>
+    <t>内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大连</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(ok) 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>继续更新郑州日盘</t>
     </r>
     <r>
       <rPr>
@@ -359,23 +329,17 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>ev</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(ok) 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新上期夜盘</t>
+      <t>so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>，和今天早上更新的</t>
     </r>
     <r>
       <rPr>
@@ -385,6 +349,94 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
+      <t>so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">一起，
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">设定手数：
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">(ok) zzsr fl34 5
+(ok) zzcf fl34 5
+(ok) zzta fl34 25
+(ok) zzsr fl36 5
+(ok) zzcf fl36 5
+(ok) zzrm fl36 4
+(ok) zzta fl36 25
+(ok) zzsr fw10 5
+(ok) zzcf fw10 5
+(ok) zzta fw10 25
+(ok) zzrm fw10 2
+(ok) zzsr fd10 4
+(ok) zzma fd10 5
+(ok) zzrm fd10 6
+(ok) zzcf fd10 4
+(ok) zzta fd10 25
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(ok) 1. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>继续更新大连日盘</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">so
 2. </t>
     </r>
@@ -396,7 +448,8 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>暂定手数</t>
+      <t xml:space="preserve">定手数
+</t>
     </r>
     <r>
       <rPr>
@@ -406,130 +459,28 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">20170214 sh night
-(ok) cu fl34 1
-(ok) cu fl36 2
-(ok) ru fl34 2
-(ok) ru fl36 2
-(ok) ru fd10 2
-(ok) ag fl34 5
-(ok) ag fl36 10
-(ok) ag fw10 2
-(ok) ag fd10 5
-(ok) zn fl34 2
-(ok) zn fl36 2
-(ok) zn fw10 1
-(ok) zn fd10 1
-(ok) al fl34 2
-(ok) al fl36 2
-(ok) rb fl34 5
-(ok) pb fl34 1
-(ok) pb fd10 1
-(ok) hc fl34 2
+      <t xml:space="preserve">(ok) dlm fl34 20
+(ok) dly fl34 2
+(ok) dla fl34 4
+(ok) dlcs fl34 6
+(ok) dljd fl34 6
+(ok) dli fl34 40
+(ok) dla fl36 1
+(ok) dlm fl36 20
+(ok) dly fl36 2
+(ok) dljd fl36 6
+(ok) dli fl36 30
+(ok) dla fw10 4
+(ok) dlm fw10 20
+(ok) dly fw10 3
+(ok) dli fw10 10
+(ok) dljd fw10 3
+(ok) dlm fd10 5
+(ok) dly fd10 3
+(ok) dli fd10 10
+(ok) dlcs fd10 6
 </t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(ok) 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新日盘上期</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>so</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">暂定手数如下：
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">20170214 sh day
-(ok) ni fl34 1
-(ok) cu fl34 2
-(ok) ru fl34 1
-(ok) ag fl34 5
-(ok) zn fl34 2
-(ok) al fl34 1
-(ok) bu fl34 1
-(ok) cu fl36 2
-(ok) ru fl36 1
-(ok) ag fl36 5
-(ok) zn fl36 2
-(ok) al fl36 2
-(ok) rb fl36 1
-(ok) cu fw10 2
-(ok) ru fw10 1
-(ok) ag fw10 5
-(ok) zn fw10 2
-(ok) rb fw10 1
-(ok) ru fd10 2
-(ok) zn fd10 2
-(ok) rb fd10 10
-(ok) pb fd10 1
-</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -733,8 +684,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F6" totalsRowShown="0">
-  <autoFilter ref="A2:F6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:F4" totalsRowShown="0">
+  <autoFilter ref="A2:F4">
     <filterColumn colId="2"/>
     <filterColumn colId="4"/>
     <filterColumn colId="5"/>
@@ -744,7 +695,7 @@
     <tableColumn id="2" name="交易所" dataDxfId="6"/>
     <tableColumn id="6" name="日/夜盘" dataDxfId="5"/>
     <tableColumn id="3" name="日期" dataDxfId="4"/>
-    <tableColumn id="4" name="：w" dataDxfId="3"/>
+    <tableColumn id="4" name="内容" dataDxfId="3"/>
     <tableColumn id="5" name="状态" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1048,10 +999,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1060,8 +1011,8 @@
     <col min="2" max="2" width="6.375" style="5" customWidth="1"/>
     <col min="3" max="3" width="8.375" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="28.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="2.25" customHeight="1">
@@ -1081,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="63" customHeight="1">
+    </row>
+    <row r="3" spans="1:6" ht="45.75" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="14" t="s">
         <v>24</v>
@@ -1096,84 +1047,40 @@
         <v>25</v>
       </c>
       <c r="D3" s="15">
-        <v>42414</v>
+        <v>42781</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="54.75" customHeight="1">
+        <v>28</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45.75" customHeight="1">
       <c r="A4" s="13"/>
       <c r="B4" s="14" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="15">
-        <v>42414</v>
+        <v>42781</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="33.75" customHeight="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="15">
-        <v>42414</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="15">
-        <v>42414</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add sc series of strategies
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -296,114 +296,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>郑州</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>夜盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>大连</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">(ok) 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新郑州夜盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">so
-2. night
-(ok) zzsr fl34 4
-(ok) zzzc fl34 1
-(ok) zzcf fl34 5
-(ok) zzta fl34 10
-(ok) zzsr fl36 5
-(ok) zzcf fl36 5
-(ok) zzrm fl36 5
-(ok) zzta fl36 10
-(ok) zzcf fw10 4
-(ok) zzrm fw10 3
-(ok) zzsr fd10 5
-(ok) zzta fd10 5
-</t>
-    </r>
+    <t>日盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锁仓测试</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(ok) 1. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新大连夜盘</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">so
-2. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">手数
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">(ok) dlm fl34 2
-(ok) dly fl34 3
-(ok) dla fl34 3
-(ok) dli fl34 10
-(ok) dla fl36 4
-(ok) dla fw10 3
-(ok) dlm fd10 5
-</t>
-    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -494,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -552,6 +457,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -970,32 +878,22 @@
         <v>26</v>
       </c>
       <c r="D3" s="15">
-        <v>42782</v>
-      </c>
-      <c r="E3" s="19" t="s">
+        <v>42787</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="52.5" customHeight="1">
       <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" s="15">
-        <v>42782</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>29</v>
-      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="13"/>

</xml_diff>

<commit_message>
Revert "update operation checklist"
This reverts commit 3d4cc13878ef101402d39dfc5a0960603f03916d.
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -300,11 +300,12 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>夜盘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新一下dli夜盘fl34的so，原来的so参数有问题</t>
+    <t>日盘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锁仓测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>passed</t>
@@ -832,7 +833,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -877,7 +878,7 @@
         <v>26</v>
       </c>
       <c r="D3" s="15">
-        <v>42788</v>
+        <v>42787</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
update shfe day strategy settings and so files
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -296,19 +296,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>大连</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>日盘</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>锁仓测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上期</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.更新上期所日盘参数
+2.更新so
+麻烦检查一下主力合约
+1. 19(ok)
+2. 63(ok)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -869,22 +873,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="52.5" customHeight="1">
+    <row r="3" spans="1:6" ht="119.25" customHeight="1">
       <c r="A3" s="13"/>
       <c r="B3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="15">
+        <v>42789</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="D3" s="15">
-        <v>42787</v>
-      </c>
-      <c r="E3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="52.5" customHeight="1">

</xml_diff>

<commit_message>
update stratrgy so files and settings for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -4,25 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
-    <sheet name="sh_19_day" sheetId="1" r:id="rId1"/>
-    <sheet name="sh_19_ngt" sheetId="3" r:id="rId2"/>
-    <sheet name="sh_63_day" sheetId="4" r:id="rId3"/>
-    <sheet name="sh_63_ngt" sheetId="5" r:id="rId4"/>
-    <sheet name="dce_day" sheetId="7" r:id="rId5"/>
-    <sheet name="dce_ngt" sheetId="6" r:id="rId6"/>
-    <sheet name="zce_day" sheetId="8" r:id="rId7"/>
-    <sheet name="zce_ngt" sheetId="9" r:id="rId8"/>
-    <sheet name="deploy new trader" sheetId="2" r:id="rId9"/>
+    <sheet name="1.sh_19_day" sheetId="1" r:id="rId1"/>
+    <sheet name="2.sh_19_ngt" sheetId="3" r:id="rId2"/>
+    <sheet name="3.sh_63_day" sheetId="4" r:id="rId3"/>
+    <sheet name="4.sh_63_ngt" sheetId="5" r:id="rId4"/>
+    <sheet name="5.dce_day" sheetId="7" r:id="rId5"/>
+    <sheet name="6.dce_ngt" sheetId="6" r:id="rId6"/>
+    <sheet name="7.zce_day" sheetId="8" r:id="rId7"/>
+    <sheet name="8.zce_ngt" sheetId="9" r:id="rId8"/>
+    <sheet name="9.deploy new trader" sheetId="2" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -261,7 +261,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>passed</t>
+    <t>状态
+(JinRui)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>状态
+(github)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -276,7 +282,7 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>更新上期夜盘的</t>
+      <t>更新大连夜盘的</t>
     </r>
     <r>
       <rPr>
@@ -296,7 +302,8 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>，</t>
+      <t xml:space="preserve">，去掉原有策略
+</t>
     </r>
     <r>
       <rPr>
@@ -306,19 +313,42 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>so_sh_night_0226.zip
-(ok)2."stra_settings_sh_night_0226.csv</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">，
-</t>
+      <t>(ok) 2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新手数</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>(ok) 1.更新郑州夜盘的so，去掉原有策略
+(ok)2.更新手数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(ok)1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新郑州日盘的</t>
     </r>
     <r>
       <rPr>
@@ -328,17 +358,17 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(ok) 3. 19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">账户
+      <t>so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -349,33 +379,34 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(ok) 4.63</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>账户</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>(ok) 1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新上期日盘的手数，</t>
+      <t>(ok) 2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">郑州日盘参数手数更新
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(ok)1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新大连日盘的</t>
     </r>
     <r>
       <rPr>
@@ -385,18 +416,17 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>stra_settings_sh_day_0226.csv
-(ok) 2. 19</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">账户
+      <t>so</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
     <r>
@@ -407,32 +437,19 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(ok) 3.63</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>账户</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>passed</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态
-(JinRui)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>状态
-(github)</t>
+      <t>(ok)2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新大连日盘参数手数
+</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -440,7 +457,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -461,8 +478,16 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -475,8 +500,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor theme="6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -495,11 +526,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -539,6 +603,30 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -546,6 +634,12 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -563,12 +657,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -594,8 +682,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:E4" totalsRowShown="0">
-  <autoFilter ref="A2:E4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:E3" insertRow="1" totalsRowShown="0">
+  <autoFilter ref="A2:E3">
     <filterColumn colId="2"/>
     <filterColumn colId="3"/>
     <filterColumn colId="4"/>
@@ -605,7 +693,7 @@
     <tableColumn id="3" name="日期" dataDxfId="5"/>
     <tableColumn id="4" name="内容" dataDxfId="4"/>
     <tableColumn id="5" name="状态_x000a_(github)" dataDxfId="3"/>
-    <tableColumn id="2" name="状态_x000a_(JinRui)" dataDxfId="0"/>
+    <tableColumn id="2" name="状态_x000a_(JinRui)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -616,8 +704,8 @@
   <autoFilter ref="A1:C37"/>
   <tableColumns count="3">
     <tableColumn id="1" name="步骤"/>
-    <tableColumn id="2" name="描述" dataDxfId="2"/>
-    <tableColumn id="3" name="备注" dataDxfId="1"/>
+    <tableColumn id="2" name="描述" dataDxfId="1"/>
+    <tableColumn id="3" name="备注" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -908,17 +996,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E4"/>
+      <selection activeCell="B2" sqref="B2:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="5.25" style="6" customWidth="1"/>
     <col min="2" max="2" width="10.375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="36.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5" style="7" customWidth="1"/>
     <col min="5" max="5" width="15.125" style="7" customWidth="1"/>
   </cols>
@@ -937,37 +1025,18 @@
         <v>21</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="71.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="10"/>
-      <c r="B3" s="11">
-        <v>42792</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>25</v>
-      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="1:5" ht="57">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11">
-        <v>42792</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1010,7 +1079,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1022,12 +1091,47 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42.75">
+      <c r="A2" s="18">
+        <v>42793</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1035,25 +1139,188 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="31.5" customHeight="1">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" customHeight="1">
+      <c r="A2" s="18">
+        <v>42793</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="18"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="18"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="18"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="18"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="18"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="18"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="18"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="27.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42.75">
+      <c r="A2" s="18">
+        <v>42793</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1061,12 +1328,47 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5">
+      <c r="A1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="48.75" customHeight="1">
+      <c r="A2" s="18">
+        <v>42793</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1076,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update miscellaneous for Explorer
</commit_message>
<xml_diff>
--- a/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
+++ b/ExplorerFund/operation/strategy_update/checklist/运维事项确认表.xlsx
@@ -4,25 +4,26 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="12765" windowHeight="5715" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="1.sh_19_day" sheetId="1" r:id="rId1"/>
     <sheet name="2.sh_19_ngt" sheetId="3" r:id="rId2"/>
     <sheet name="3.sh_63_day" sheetId="4" r:id="rId3"/>
     <sheet name="4.sh_63_ngt" sheetId="5" r:id="rId4"/>
-    <sheet name="5.dce_day" sheetId="7" r:id="rId5"/>
-    <sheet name="6.dce_ngt" sheetId="6" r:id="rId6"/>
-    <sheet name="7.zce_day" sheetId="8" r:id="rId7"/>
-    <sheet name="8.zce_ngt" sheetId="9" r:id="rId8"/>
-    <sheet name="9.deploy new trader" sheetId="2" r:id="rId9"/>
+    <sheet name="sh_85_day" sheetId="10" r:id="rId5"/>
+    <sheet name="5.dce_day" sheetId="7" r:id="rId6"/>
+    <sheet name="6.dce_ngt" sheetId="6" r:id="rId7"/>
+    <sheet name="7.zce_day" sheetId="8" r:id="rId8"/>
+    <sheet name="8.zce_ngt" sheetId="9" r:id="rId9"/>
+    <sheet name="9.deploy new trader" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -332,23 +333,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(ok) 1.更新郑州夜盘的so，去掉原有策略
-(ok)2.更新手数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>(ok)1.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>更新大连日盘的</t>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>明天日盘铁矿石</t>
     </r>
     <r>
       <rPr>
@@ -358,17 +355,34 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>so</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
+      <t>i</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">加为半仓
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(ok)1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新上期日盘参数手数
 </t>
     </r>
     <r>
@@ -389,15 +403,26 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">更新大连日盘参数手数
+      <t xml:space="preserve">更新so
 </t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>明天dli日盘策略手数继续减半</t>
-  </si>
-  <si>
+    <r>
+      <t>(ok)1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新上期日盘参数手数
+</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -406,6 +431,27 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
+      <t>(ok)2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新so
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>(ok)1.</t>
     </r>
     <r>
@@ -416,7 +462,8 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>明天测试日盘</t>
+      <t xml:space="preserve">更新上期夜盘参数手数
+</t>
     </r>
     <r>
       <rPr>
@@ -426,17 +473,35 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>dli</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>，</t>
+      <t>(ok)2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新so
+</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>(ok)1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新上期夜盘参数手数
+</t>
     </r>
     <r>
       <rPr>
@@ -446,19 +511,32 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>fl34s</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">策略，一手
+      <t>(ok)2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新so
 </t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新郑州夜盘
+(ok)1.so
+(ok)2.和手数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>passed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -467,7 +545,38 @@
         <family val="2"/>
         <charset val="134"/>
       </rPr>
-      <t>(ok) 2.so</t>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">更新郑州日盘参数
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>更新手数</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -586,7 +695,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -620,9 +729,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -680,6 +786,16 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="6"/>
+        </right>
+        <top style="thin">
+          <color theme="6"/>
+        </top>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
@@ -705,7 +821,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:E3" insertRow="1" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A2:E3" totalsRowShown="0">
   <autoFilter ref="A2:E3">
     <filterColumn colId="2"/>
     <filterColumn colId="3"/>
@@ -1021,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1054,12 +1170,20 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" ht="42.75">
       <c r="A3" s="10"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
+      <c r="B3" s="11">
+        <v>42802</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1071,48 +1195,132 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="23.75" style="7" customWidth="1"/>
+    <col min="3" max="3" width="33.875" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="63.75" customHeight="1">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18" customHeight="1">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18" customHeight="1">
+      <c r="B5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18" customHeight="1">
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" customHeight="1">
+      <c r="B7" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18" customHeight="1">
+      <c r="B8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17.25" customHeight="1">
+      <c r="B10" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" customHeight="1">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="17.25" customHeight="1">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="41.25">
+      <c r="B13" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1122,36 +1330,148 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="10.75" customWidth="1"/>
+    <col min="4" max="4" width="10.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="27">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="60" customHeight="1">
+      <c r="A2" s="17">
+        <v>42802</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="56.25">
+      <c r="A1" s="17">
+        <v>42802</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="2" max="2" width="36.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="42.75">
-      <c r="A2" s="18">
-        <v>42793</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>25</v>
+      <c r="A2" s="17">
+        <v>42802</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1161,6 +1481,55 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="40.5">
+      <c r="A1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.5">
+      <c r="A2" s="17">
+        <v>42800</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D17"/>
   <sheetViews>
@@ -1177,122 +1546,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="31.5" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="45" customHeight="1">
-      <c r="A2" s="18">
+      <c r="A2" s="17">
         <v>42793</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="18"/>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
     </row>
     <row r="12" spans="1:4">
-      <c r="A12" s="18"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="A12" s="17"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="18"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="18"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="18"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="A16" s="17"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="18"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1301,12 +1670,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1316,45 +1685,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.5" customHeight="1">
-      <c r="A2" s="18">
-        <v>42795</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="18">
-        <v>42795</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>25</v>
+      <c r="A2" s="17">
+        <v>42802</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1364,7 +1719,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -1379,160 +1734,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="40.5">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="48.75" customHeight="1">
-      <c r="A2" s="18">
-        <v>42793</v>
-      </c>
-      <c r="B2" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>25</v>
+      <c r="A2" s="17">
+        <v>42802</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
-  <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="23.75" style="7" customWidth="1"/>
-    <col min="3" max="3" width="33.875" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="63.75" customHeight="1">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="18" customHeight="1">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="18" customHeight="1">
-      <c r="B5" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18" customHeight="1">
-      <c r="B6" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18" customHeight="1">
-      <c r="B7" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="18" customHeight="1">
-      <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.25" customHeight="1">
-      <c r="B10" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A12">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="41.25">
-      <c r="B13" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>